<commit_message>
cosine similarity to compare condition
</commit_message>
<xml_diff>
--- a/src/main/resources/data/descript.xlsx
+++ b/src/main/resources/data/descript.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanh2\IdeaProjects\selenium\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278AB88F-DFC3-410F-B446-7A119E3EEE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C8C6BC-E39C-4932-875D-69CF8F5E3625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -145,67 +145,6 @@
   <si>
     <t>4.1. Log in successfully. New page is opened with title is "Dashboard"
 4.2. Exist "Dashboard" , "Posts", "Media", "Comments", "Tools", "Collapse menu"</t>
-  </si>
-  <si>
-    <t>Logout_001</t>
-  </si>
-  <si>
-    <t>Check logout successfully</t>
-  </si>
-  <si>
-    <t>1. User must be login successfully into the system</t>
-  </si>
-  <si>
-    <t>1. Hover over the account's avatar in the upper right corner of the screen
-2. Click "Log out" button</t>
-  </si>
-  <si>
-    <t>1. Display submenu. Exist: "Edit My Profile", "Log Out"
-2. Log out successfully. Dirrect to "Login" page with message: "You are now logged out."</t>
-  </si>
-  <si>
-    <t>AddPost_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add new post </t>
-  </si>
-  <si>
-    <t>1. Click "Posts" item in left menu 
-2. Click "Add New" item 
-3. Fill "TitleTestRanorex" into "Enter title here" placeholder
-4. Fill "Test creating new post" into text-area 
-5. Click "Publish" button
-6. Click "View post" hyper link</t>
-  </si>
-  <si>
-    <t>1. "Posts" page is opened
-5. New post is created successfully: 
-- Page change to "Edit Post"
-- Display "Post published. View post" 
-6. Navigate to new post</t>
-  </si>
-  <si>
-    <t>FilterPost_001</t>
-  </si>
-  <si>
-    <t>Filter posts</t>
-  </si>
-  <si>
-    <t>1. User must be login successfully into the system
-2. Exist posts which are uncategoried and created in November 2023</t>
-  </si>
-  <si>
-    <t>1. Click "Posts" item in left menu 
-2. Click "All" hyper link 
-3. In second listbox: Select "November 2023" item
-4. In third listbox: Select "Uncategoried" list box
-5. Click "Filter" button</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. "All" Click is selected 
-3. "November 2023" item is selected
-4. "Uncategoried" is selected
-5. Clickle load only tiems which ared created in November 2023 and uncategoried </t>
   </si>
 </sst>
 </file>
@@ -246,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -255,73 +194,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color indexed="8"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -329,36 +212,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -640,192 +508,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B321DB5-ACAE-4B80-87E9-BA1668DA7C70}">
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <cols>
-    <col min="4" max="4" width="33.44140625" customWidth="1"/>
-    <col min="5" max="5" width="42.5546875" customWidth="1"/>
-    <col min="6" max="6" width="25.44140625" customWidth="1"/>
-    <col min="7" max="7" width="22.77734375" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.6">
+    <row r="1" spans="1:6" ht="30.6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2"/>
     </row>
-    <row r="2" spans="1:8" ht="51" customHeight="1">
+    <row r="2" spans="1:6" ht="204">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="51" customHeight="1">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:6" ht="295.8">
+      <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="5"/>
     </row>
-    <row r="4" spans="1:8" ht="20.399999999999999" customHeight="1">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:6" ht="193.8">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="40.799999999999997" customHeight="1">
-      <c r="A5" s="8" t="s">
+    <row r="5" spans="1:6" ht="193.8">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="1:8" ht="40.799999999999997" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="1:8" ht="20.399999999999999" customHeight="1">
-      <c r="A7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" ht="20.399999999999999" customHeight="1">
-      <c r="A8" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="5"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="C2:C8" xr:uid="{E0BF91BC-1845-410A-AE55-3E9CDA237F6A}">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C5" xr:uid="{E0BF91BC-1845-410A-AE55-3E9CDA237F6A}">
       <formula1>"Normal,Abnormal"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>